<commit_message>
Sofia | test 1 id fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CBE1A9-7F6F-4645-856D-659C964CD191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C7DEE-159C-495C-A2D8-F40C52A008C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7650" yWindow="2100" windowWidth="21600" windowHeight="11385" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="18" r:id="rId1"/>
@@ -621,7 +621,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Sofia | Wintage fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8C7DEE-159C-495C-A2D8-F40C52A008C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2D8A0A-6BDC-4FEA-B092-64BA234BEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="2100" windowWidth="21600" windowHeight="11385" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="18" r:id="rId1"/>
@@ -621,7 +621,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
sofia | general | translate | added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2D8A0A-6BDC-4FEA-B092-64BA234BEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4433DB78-C652-47AC-BDD8-7D0288966F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="18" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
   <si>
     <t>L [mm]</t>
   </si>
@@ -225,18 +225,62 @@
   </si>
   <si>
     <t>m^2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>ValueEN</t>
+  </si>
+  <si>
+    <t>ValueRU</t>
+  </si>
+  <si>
+    <t>Неограниченный</t>
+  </si>
+  <si>
+    <t>София</t>
+  </si>
+  <si>
+    <t>Судно, предназначенное для перевозки сухих генеральных грузов</t>
+  </si>
+  <si>
+    <t>Новороссийск</t>
+  </si>
+  <si>
+    <t>Российская Федерация</t>
+  </si>
+  <si>
+    <t>Вестербрук, Нидерланды</t>
+  </si>
+  <si>
+    <t>ООО "Кубанская морская компания"</t>
+  </si>
+  <si>
+    <t>РС</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,14 +353,14 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,12 +368,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -618,406 +665,517 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F73F37-6A3E-4306-8718-2CD1213133A8}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="64" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5">
         <v>506</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
-        <v>130.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="5">
-        <v>138.86000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>130.5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="5">
-        <v>15.87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>138.86000000000001</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="5">
-        <v>11.15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>15.87</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="5">
+        <v>11.15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="5">
         <v>65.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75">
-      <c r="A11" s="4" t="s">
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5">
         <v>9245263</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="4" t="s">
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75">
+      <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75">
-      <c r="A14" s="4" t="s">
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75">
+      <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1">
         <v>273251830</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C16" s="5">
         <v>3230.55</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="5">
-        <v>59.837000000000003</v>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="5">
-        <v>7.81</v>
+        <v>59.837000000000003</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="5">
-        <v>-0.44</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>7.81</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="5">
-        <v>2.0009999999999999</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>-0.44</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="5">
-        <v>4.3079999999999998</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="5">
-        <v>68.819999999999993</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>4.3079999999999998</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="5">
-        <v>27.78</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>68.819999999999993</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="5">
-        <v>7.9969999999999999</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>27.78</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="5">
-        <v>4.6529999999999996</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>7.9969999999999999</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="5">
+        <v>4.6529999999999996</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="5">
-        <v>82</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="C27" s="5">
-        <v>-0.65249999999999997</v>
-      </c>
-      <c r="D27" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="5">
-        <v>0.65249999999999997</v>
-      </c>
-      <c r="D28" s="1"/>
+        <v>-0.65249999999999997</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C29" s="5">
-        <v>10890</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>0.65249999999999997</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="5">
+        <v>10890</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C33" s="1">
         <v>2002</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="D33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="D34" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="D35" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="D36" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{81732E85-6C1A-4CD5-B0D3-7F8746370AFD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{81732E85-6C1A-4CD5-B0D3-7F8746370AFD}">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>Unrestricted,R1,R2,R2-RSN,"R2-RSN(4,5)",R3-RSN,R3</x12ac:list>

</xml_diff>

<commit_message>
sofia | speed added
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/SSS_Sofia_General.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95861988-D2FF-4352-8532-26C85C0FE20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA074BF-583A-43BA-B9C7-5EA0E734F611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="797" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="18" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="77">
   <si>
     <t>L [mm]</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>РС</t>
+  </si>
+  <si>
+    <t>knot</t>
+  </si>
+  <si>
+    <t>Operational speed</t>
   </si>
 </sst>
 </file>
@@ -665,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F73F37-6A3E-4306-8718-2CD1213133A8}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1171,6 +1177,17 @@
       </c>
       <c r="D37" s="7" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="1">
+        <v>14.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>